<commit_message>
Updated Soulbinds based on Beta Build 32694, Generated Profiles
</commit_message>
<xml_diff>
--- a/covenants/Soulbinds.xlsx
+++ b/covenants/Soulbinds.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spung\repos\simc-profiles\covenants\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SpanierTh\source\repos\simc-profiles\covenants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03226D5-6E2F-4A10-92EF-9ABBAC321452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="SoulbindAbilities" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Legendaries!$A$1:$H$88</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SoulbindAbilities!$A$1:$J$177</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="1413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="1413">
   <si>
     <t>pc</t>
   </si>
@@ -4287,7 +4286,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4633,11 +4632,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4833,11 +4832,11 @@
         <v>175</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>319982,MAOne,Move As One,sb,3,0,Draven,Draven_end1,0</v>
+        <v>319982,MAOne,Move As One,sb,3,0,Draven,Draven_end1,1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -6052,13 +6051,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>1091</v>
+        <v>1102</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C46" t="s">
-        <v>1181</v>
+        <v>1192</v>
       </c>
       <c r="D46" t="s">
         <v>4</v>
@@ -6076,19 +6075,19 @@
         <v>0</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" si="0"/>
-        <v>331609,FFilter,Forgelite Filter,sb,1,0,Forgelite,,0</v>
+        <f>CONCATENATE(A46,",",B46,",",C46,",",D46,",",E46,",",F46,",",G46,",",H46,",",I46)</f>
+        <v>333950,BCtAction,Bron's Call to Action,sb,1,0,Forgelite,,0</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="D47" t="s">
         <v>4</v>
@@ -6103,22 +6102,22 @@
         <v>100</v>
       </c>
       <c r="I47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="str">
-        <f t="shared" si="0"/>
-        <v>331610,CAdditive,Charged Additive,sb,2,0,Forgelite,,1</v>
+        <f>CONCATENATE(A47,",",B47,",",C47,",",D47,",",E47,",",F47,",",G47,",",H47,",",I47)</f>
+        <v>331609,FFilter,Forgelite Filter,sb,2,0,Forgelite,,0</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>1102</v>
+        <v>1092</v>
       </c>
       <c r="B48" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>1192</v>
+        <v>1182</v>
       </c>
       <c r="D48" t="s">
         <v>4</v>
@@ -6133,11 +6132,11 @@
         <v>100</v>
       </c>
       <c r="I48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" si="0"/>
-        <v>333950,BCtAction,Bron's Call to Action,sb,2,0,Forgelite,,0</v>
+        <f>CONCATENATE(A48,",",B48,",",C48,",",D48,",",E48,",",F48,",",G48,",",H48,",",I48)</f>
+        <v>331610,CAdditive,Charged Additive,sb,2,0,Forgelite,,1</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -6169,7 +6168,7 @@
         <v>0</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A49,",",B49,",",C49,",",D49,",",E49,",",F49,",",G49,",",H49,",",I49)</f>
         <v>Forgelite_end1,Forgelite_end1,Endurance Conduit,ec,3,0,Forgelite,331610,0</v>
       </c>
     </row>
@@ -6202,7 +6201,7 @@
         <v>0</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A50,",",B50,",",C50,",",D50,",",E50,",",F50,",",G50,",",H50,",",I50)</f>
         <v>Forgelite_pot1,Forgelite_pot1,Potency Conduit,pc,3,0,Forgelite,331609,0</v>
       </c>
     </row>
@@ -6232,7 +6231,7 @@
         <v>0</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A51,",",B51,",",C51,",",D51,",",E51,",",F51,",",G51,",",H51,",",I51)</f>
         <v>Forgelite_fin1,Forgelite_fin1,Finesse Conduit,fc,4,0,Forgelite,,0</v>
       </c>
     </row>
@@ -6262,7 +6261,7 @@
         <v>0</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A52,",",B52,",",C52,",",D52,",",E52,",",F52,",",G52,",",H52,",",I52)</f>
         <v>331725,RPlumage,Resilient Plumage,sb,5,0,Forgelite,,0</v>
       </c>
     </row>
@@ -6292,7 +6291,7 @@
         <v>1</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A53,",",B53,",",C53,",",D53,",",E53,",",F53,",",G53,",",H53,",",I53)</f>
         <v>331726,RMaterials,Regenerating Materials,sb,5,0,Forgelite,,1</v>
       </c>
     </row>
@@ -6323,7 +6322,7 @@
         <v>0</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A54,",",B54,",",C54,",",D54,",",E54,",",F54,",",G54,",",H54,",",I54)</f>
         <v>Forgelite_end2,Forgelite_end2,Endurance Conduit,ec,6,0,Forgelite,,0</v>
       </c>
     </row>
@@ -6354,7 +6353,7 @@
         <v>0</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A55,",",B55,",",C55,",",D55,",",E55,",",F55,",",G55,",",H55,",",I55)</f>
         <v>Forgelite_fin2,Forgelite_fin2,Finesse Conduit,fc,7,29,Forgelite,,0</v>
       </c>
     </row>
@@ -6385,7 +6384,7 @@
         <v>0</v>
       </c>
       <c r="J56" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A56,",",B56,",",C56,",",D56,",",E56,",",F56,",",G56,",",H56,",",I56)</f>
         <v>Forgelite_pot2,Forgelite_pot2,Potency Conduit,pc,7,29,Forgelite,,0</v>
       </c>
     </row>
@@ -6416,7 +6415,7 @@
         <v>0</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A57,",",B57,",",C57,",",D57,",",E57,",",F57,",",G57,",",H57,",",I57)</f>
         <v>Forgelite_end3,Forgelite_end3,Endurance Conduit,ec,7,29,Forgelite,,0</v>
       </c>
     </row>
@@ -6449,7 +6448,7 @@
         <v>0</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A58,",",B58,",",C58,",",D58,",",E58,",",F58,",",G58,",",H58,",",I58)</f>
         <v>331611,SClamps,Soulsteel Clamps,sb,8,31,Forgelite,Forgelite_pot2,0</v>
       </c>
     </row>
@@ -6482,7 +6481,7 @@
         <v>1</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A59,",",B59,",",C59,",",D59,",",E59,",",F59,",",G59,",",H59,",",I59)</f>
         <v>331612,SDCore,Sparkling Driftglobe Core,sb,8,31,Forgelite,Forgelite_fin2,1</v>
       </c>
     </row>
@@ -6515,7 +6514,7 @@
         <v>0</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" si="0"/>
+        <f>CONCATENATE(A60,",",B60,",",C60,",",D60,",",E60,",",F60,",",G60,",",H60,",",I60)</f>
         <v>333935,HoGenesis,Hammer of Genesis,sb,8,31,Forgelite,Forgelite_end3,0</v>
       </c>
     </row>
@@ -7481,22 +7480,22 @@
         <v>0</v>
       </c>
       <c r="J91" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A91,",",B91,",",C91,",",D91,",",E91,",",F91,",",G91,",",H91,",",I91)</f>
         <v>325066,WHTactics,Wild Hunt Tactics,sb,1,0,Korayn,,0</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>1054</v>
+        <v>154</v>
       </c>
       <c r="B92" t="s">
-        <v>35</v>
+        <v>154</v>
       </c>
       <c r="C92" t="s">
-        <v>1144</v>
+        <v>1206</v>
       </c>
       <c r="D92" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E92">
         <v>2</v>
@@ -7507,26 +7506,27 @@
       <c r="G92" t="s">
         <v>181</v>
       </c>
+      <c r="H92" s="1"/>
       <c r="I92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J92" t="str">
-        <f t="shared" si="1"/>
-        <v>325065,WHCharge,Wild Hunt's Charge,sb,2,0,Korayn,,1</v>
+        <f>CONCATENATE(A92,",",B92,",",C92,",",D92,",",E92,",",F92,",",G92,",",H92,",",I92)</f>
+        <v>Koryan_pot1,Koryan_pot1,Potency Conduit,pc,2,0,Korayn,,0</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>1056</v>
+        <v>158</v>
       </c>
       <c r="B93" t="s">
-        <v>37</v>
+        <v>158</v>
       </c>
       <c r="C93" t="s">
-        <v>1146</v>
+        <v>1205</v>
       </c>
       <c r="D93" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E93">
         <v>2</v>
@@ -7541,22 +7541,22 @@
         <v>0</v>
       </c>
       <c r="J93" t="str">
-        <f t="shared" si="1"/>
-        <v>325067,HotWH,Horn of the Wild Hunt,sb,2,0,Korayn,,0</v>
+        <f>CONCATENATE(A93,",",B93,",",C93,",",D93,",",E93,",",F93,",",G93,",",H93,",",I93)</f>
+        <v>Koryan_end1,Koryan_end1,Endurance Conduit,ec,2,0,Korayn,,0</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>156</v>
+        <v>1054</v>
       </c>
       <c r="B94" t="s">
-        <v>156</v>
+        <v>35</v>
       </c>
       <c r="C94" t="s">
-        <v>1207</v>
+        <v>1144</v>
       </c>
       <c r="D94" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E94">
         <v>3</v>
@@ -7567,29 +7567,29 @@
       <c r="G94" t="s">
         <v>181</v>
       </c>
-      <c r="H94" s="1">
-        <v>325065</v>
+      <c r="H94" t="s">
+        <v>158</v>
       </c>
       <c r="I94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J94" t="str">
-        <f t="shared" si="1"/>
-        <v>Koryan_fin1,Koryan_fin1,Finesse Conduit,fc,3,0,Korayn,325065,0</v>
+        <f>CONCATENATE(A94,",",B94,",",C94,",",D94,",",E94,",",F94,",",G94,",",H94,",",I94)</f>
+        <v>325065,WHCharge,Wild Hunt's Charge,sb,3,0,Korayn,Koryan_end1,1</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>154</v>
+        <v>1056</v>
       </c>
       <c r="B95" t="s">
-        <v>154</v>
+        <v>37</v>
       </c>
       <c r="C95" t="s">
-        <v>1206</v>
+        <v>1146</v>
       </c>
       <c r="D95" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E95">
         <v>3</v>
@@ -7600,29 +7600,29 @@
       <c r="G95" t="s">
         <v>181</v>
       </c>
-      <c r="H95" s="1">
-        <v>325067</v>
+      <c r="H95" t="s">
+        <v>154</v>
       </c>
       <c r="I95">
         <v>0</v>
       </c>
       <c r="J95" t="str">
-        <f t="shared" si="1"/>
-        <v>Koryan_pot1,Koryan_pot1,Potency Conduit,pc,3,0,Korayn,325067,0</v>
+        <f>CONCATENATE(A95,",",B95,",",C95,",",D95,",",E95,",",F95,",",G95,",",H95,",",I95)</f>
+        <v>325067,HotWH,Horn of the Wild Hunt,sb,3,0,Korayn,Koryan_pot1,0</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B96" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C96" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
       <c r="D96" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E96">
         <v>4</v>
@@ -7633,12 +7633,13 @@
       <c r="G96" t="s">
         <v>181</v>
       </c>
+      <c r="H96" s="1"/>
       <c r="I96">
         <v>0</v>
       </c>
       <c r="J96" t="str">
-        <f t="shared" si="1"/>
-        <v>Koryan_end1,Koryan_end1,Endurance Conduit,ec,4,0,Korayn,,0</v>
+        <f>CONCATENATE(A96,",",B96,",",C96,",",D96,",",E96,",",F96,",",G96,",",H96,",",I96)</f>
+        <v>Koryan_fin1,Koryan_fin1,Finesse Conduit,fc,4,0,Korayn,,0</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -7667,7 +7668,7 @@
         <v>1</v>
       </c>
       <c r="J97" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A97,",",B97,",",C97,",",D97,",",E97,",",F97,",",G97,",",H97,",",I97)</f>
         <v>325072,VSTechn,Vorkai Sharpening Techniques,sb,5,0,Korayn,,1</v>
       </c>
     </row>
@@ -7697,7 +7698,7 @@
         <v>0</v>
       </c>
       <c r="J98" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A98,",",B98,",",C98,",",D98,",",E98,",",F98,",",G98,",",H98,",",I98)</f>
         <v>325073,GIForm,Get In Formation,sb,5,0,Korayn,,0</v>
       </c>
     </row>
@@ -7728,7 +7729,7 @@
         <v>0</v>
       </c>
       <c r="J99" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A99,",",B99,",",C99,",",D99,",",E99,",",F99,",",G99,",",H99,",",I99)</f>
         <v>Koryan_end2,Koryan_end2,Endurance Conduit,ec,6,0,Korayn,,0</v>
       </c>
     </row>
@@ -7759,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="J100" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A100,",",B100,",",C100,",",D100,",",E100,",",F100,",",G100,",",H100,",",I100)</f>
         <v>Koryan_fin2,Koryan_fin2,Finesse Conduit,fc,7,28,Korayn,,0</v>
       </c>
     </row>
@@ -7790,7 +7791,7 @@
         <v>0</v>
       </c>
       <c r="J101" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A101,",",B101,",",C101,",",D101,",",E101,",",F101,",",G101,",",H101,",",I101)</f>
         <v>Koryan_pot2,Koryan_pot2,Potency Conduit,pc,7,28,Korayn,,0</v>
       </c>
     </row>
@@ -7820,7 +7821,7 @@
         <v>0</v>
       </c>
       <c r="J102" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A102,",",B102,",",C102,",",D102,",",E102,",",F102,",",G102,",",H102,",",I102)</f>
         <v>Koryan_end3,Koryan_end3,Endurance Conduit,ec,7,28,Korayn,,0</v>
       </c>
     </row>
@@ -7853,7 +7854,7 @@
         <v>0</v>
       </c>
       <c r="J103" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A103,",",B103,",",C103,",",D103,",",E103,",",F103,",",G103,",",H103,",",I103)</f>
         <v>325068,FYFoes,Face Your Foes,sb,8,31,Korayn,Koryan_pot2,0</v>
       </c>
     </row>
@@ -7886,7 +7887,7 @@
         <v>0</v>
       </c>
       <c r="J104" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A104,",",B104,",",C104,",",D104,",",E104,",",F104,",",G104,",",H104,",",I104)</f>
         <v>325069,FStrike,First Strike,sb,8,31,Korayn,Koryan_end3,0</v>
       </c>
     </row>
@@ -7919,7 +7920,7 @@
         <v>1</v>
       </c>
       <c r="J105" t="str">
-        <f t="shared" si="1"/>
+        <f>CONCATENATE(A105,",",B105,",",C105,",",D105,",",E105,",",F105,",",G105,",",H105,",",I105)</f>
         <v>325601,HtLine,Hold the Line,sb,8,31,Korayn,Koryan_fin2,1</v>
       </c>
     </row>
@@ -10161,13 +10162,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J177" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J16">
+  <autoFilter ref="A1:J177">
+    <sortState ref="A91:J105">
       <sortCondition ref="G2:G177"/>
       <sortCondition ref="E2:E177"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G177">
+  <sortState ref="A2:G177">
     <sortCondition ref="G2:G177"/>
     <sortCondition ref="E2:E177"/>
   </sortState>
@@ -10176,12 +10177,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K274"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10459,11 +10460,11 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
-        <v>18,336472,Shivering Core,SC,Mage,Frost,pc,0,0,1</v>
+        <v>18,336472,Shivering Core,SC,Mage,Frost,pc,0,0,0</v>
       </c>
     </row>
     <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -10540,7 +10541,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -10550,7 +10551,7 @@
       </c>
       <c r="K17" t="str">
         <f t="shared" si="2"/>
-        <v>21,336569,Ice Bite,IB,Mage,Frost,pc,1,0,0</v>
+        <v>21,336569,Ice Bite,IB,Mage,Frost,pc,0,0,0</v>
       </c>
     </row>
     <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -10774,11 +10775,11 @@
         <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" t="str">
         <f>CONCATENATE(A28,",",B28,",",C28,",",D28,",",E28,",",F28,",",G28,",",H28,",",I28,",",J28)</f>
-        <v>32,336852,Master Flame,MF,Mage,Fire,pc,0,0,1</v>
+        <v>32,336852,Master Flame,MF,Mage,Fire,pc,0,0,0</v>
       </c>
     </row>
     <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -14559,7 +14560,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K274" xr:uid="{00000000-0009-0000-0000-000001000000}">
+  <autoFilter ref="A1:K274">
     <filterColumn colId="3">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -14571,7 +14572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14786,7 +14787,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14861,7 +14862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A072932B-80A9-4BEA-888B-75EEB782215E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17522,7 +17523,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H88" xr:uid="{6CD2DD87-6A66-490B-93FA-A0BEBCC21442}"/>
+  <autoFilter ref="A1:H88"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>